<commit_message>
Se agrego cambio de contraseña, se cambio el logo y se agrego modificar preguntas
</commit_message>
<xml_diff>
--- a/ServiceDesk.xlsx
+++ b/ServiceDesk.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="4" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Servicios" sheetId="1" r:id="rId4"/>
@@ -1435,7 +1435,7 @@
   </sheetPr>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -2199,7 +2199,7 @@
   </sheetPr>
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>